<commit_message>
retour à github - memory usage reduction - pandas profiling report - Filtering unimportant columns - Dropping inoperable columns (code, product_name, quantity, brands) -- beaucoup de travail sur la colonne quantity (clustering)
</commit_message>
<xml_diff>
--- a/data-fields.xlsx
+++ b/data-fields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="30" windowWidth="15150" windowHeight="8520" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="5340" yWindow="30" windowWidth="15150" windowHeight="8520" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="data-fields (fichier txt orig)" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="comp real col &amp; data-fields" sheetId="2" r:id="rId3"/>
     <sheet name="Feuil1" sheetId="4" r:id="rId4"/>
     <sheet name="colonnes-missing_val" sheetId="5" r:id="rId5"/>
+    <sheet name="IMPRESSION" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="773">
   <si>
     <t>This file describes the fields from the CSV export of the products in the Open Food Facts database.</t>
   </si>
@@ -2343,7 +2344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2542,6 +2543,13 @@
     <font>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2918,7 +2926,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2974,6 +2982,8 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4150,8 +4160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:A176"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4951,8 +4961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,7 +4987,7 @@
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="13" t="s">
         <v>159</v>
       </c>
       <c r="C2" t="s">
@@ -4988,7 +4998,7 @@
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="13" t="s">
         <v>160</v>
       </c>
       <c r="C3" t="s">
@@ -5054,7 +5064,7 @@
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="13" t="s">
         <v>165</v>
       </c>
       <c r="C9" t="s">
@@ -5065,7 +5075,7 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
@@ -5076,7 +5086,7 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>166</v>
       </c>
       <c r="C11" t="s">
@@ -6776,8 +6786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7654,7 +7664,7 @@
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="8"/>
-      <c r="D144" s="14" t="s">
+      <c r="C144" s="14" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7859,8 +7869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11192,4 +11202,788 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C175"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>